<commit_message>
Atualizando Planejamento Release - UC02 #12 - UC03 #13
</commit_message>
<xml_diff>
--- a/Artefatos/Planejamento de Release.xlsx
+++ b/Artefatos/Planejamento de Release.xlsx
@@ -187,7 +187,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -349,43 +349,8 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -405,7 +370,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -450,6 +415,33 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -464,39 +456,8 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -816,7 +777,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -828,24 +789,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="20" t="s">
+      <c r="B1" s="34"/>
+      <c r="C1" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="21"/>
-      <c r="E1" s="22" t="s">
+      <c r="D1" s="34"/>
+      <c r="E1" s="35" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="25" t="s">
+      <c r="G1" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="21"/>
+      <c r="H1" s="34"/>
     </row>
     <row r="2" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
@@ -860,7 +821,7 @@
       <c r="D2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="23"/>
+      <c r="E2" s="36"/>
       <c r="F2" s="5" t="s">
         <v>9</v>
       </c>
@@ -879,32 +840,38 @@
       <c r="B3" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="41">
-        <v>42683</v>
-      </c>
-      <c r="D3" s="41">
-        <v>42689</v>
+      <c r="C3" s="32">
+        <v>42690</v>
+      </c>
+      <c r="D3" s="32">
+        <v>42704</v>
       </c>
       <c r="E3" s="11">
         <v>6</v>
       </c>
-      <c r="F3" s="29"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="36"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="26"/>
     </row>
     <row r="4" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="38"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="34"/>
-      <c r="H4" s="37"/>
+      <c r="C4" s="31">
+        <v>42683</v>
+      </c>
+      <c r="D4" s="31">
+        <v>42689</v>
+      </c>
+      <c r="E4" s="8">
+        <v>6</v>
+      </c>
+      <c r="F4" s="40"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="27"/>
     </row>
     <row r="5" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
@@ -913,12 +880,18 @@
       <c r="B5" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="38"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="34"/>
-      <c r="H5" s="37"/>
+      <c r="C5" s="31">
+        <v>42683</v>
+      </c>
+      <c r="D5" s="31">
+        <v>42689</v>
+      </c>
+      <c r="E5" s="8">
+        <v>6</v>
+      </c>
+      <c r="F5" s="40"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="27"/>
     </row>
     <row r="6" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
@@ -927,12 +900,18 @@
       <c r="B6" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="34"/>
-      <c r="H6" s="37"/>
+      <c r="C6" s="32">
+        <v>42705</v>
+      </c>
+      <c r="D6" s="32">
+        <v>42723</v>
+      </c>
+      <c r="E6" s="11">
+        <v>17</v>
+      </c>
+      <c r="F6" s="23"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="10"/>
     </row>
     <row r="7" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
@@ -941,12 +920,12 @@
       <c r="B7" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="38"/>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
-      <c r="F7" s="32"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="37"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="27"/>
     </row>
     <row r="8" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
@@ -955,12 +934,12 @@
       <c r="B8" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="38"/>
-      <c r="D8" s="38"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="32"/>
-      <c r="G8" s="35"/>
-      <c r="H8" s="37"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="27"/>
     </row>
     <row r="9" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
@@ -969,16 +948,11 @@
       <c r="B9" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="42">
-        <v>42690</v>
-      </c>
-      <c r="D9" s="42">
-        <v>42704</v>
-      </c>
-      <c r="E9" s="38"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="37"/>
+      <c r="C9" s="28"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="27"/>
     </row>
     <row r="10" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
@@ -987,16 +961,12 @@
       <c r="B10" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="42">
-        <v>42690</v>
-      </c>
-      <c r="D10" s="42">
-        <v>42704</v>
-      </c>
-      <c r="E10" s="38"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="28"/>
-      <c r="H10" s="37"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="27"/>
     </row>
     <row r="11" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
@@ -1005,16 +975,12 @@
       <c r="B11" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="42">
-        <v>42705</v>
-      </c>
-      <c r="D11" s="42">
-        <v>42723</v>
-      </c>
-      <c r="E11" s="39"/>
-      <c r="F11" s="32"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="10"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="21"/>
+      <c r="H11" s="27"/>
     </row>
     <row r="12" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">
@@ -1023,9 +989,9 @@
       <c r="B12" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="38"/>
-      <c r="D12" s="38"/>
-      <c r="E12" s="38"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
       <c r="F12" s="14"/>
       <c r="G12" s="15"/>
       <c r="H12" s="14"/>
@@ -1037,9 +1003,9 @@
       <c r="B13" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="38"/>
-      <c r="D13" s="38"/>
-      <c r="E13" s="38"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
       <c r="F13" s="14"/>
       <c r="G13" s="15"/>
       <c r="H13" s="14"/>
@@ -1051,9 +1017,9 @@
       <c r="B14" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="38"/>
-      <c r="D14" s="38"/>
-      <c r="E14" s="38"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
       <c r="F14" s="14"/>
       <c r="G14" s="15"/>
       <c r="H14" s="14"/>
@@ -1065,9 +1031,9 @@
       <c r="B15" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="38"/>
-      <c r="D15" s="38"/>
-      <c r="E15" s="38"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
       <c r="F15" s="14"/>
       <c r="G15" s="15"/>
       <c r="H15" s="14"/>
@@ -1079,9 +1045,9 @@
       <c r="B16" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="40"/>
-      <c r="D16" s="40"/>
-      <c r="E16" s="40"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
       <c r="F16" s="18"/>
       <c r="G16" s="19"/>
       <c r="H16" s="18"/>

</xml_diff>

<commit_message>
#16-Organizacao da pasta de artefatos
</commit_message>
<xml_diff>
--- a/Artefatos/Planejamento de Release.xlsx
+++ b/Artefatos/Planejamento de Release.xlsx
@@ -1,20 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27610"/>
+  <workbookPr checkCompatibility="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Marielen\Documents\Engenharia de Software\Venezuela\Artefatos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/igorpgcosta/Downloads/Venezuela/Artefatos/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14620"/>
   </bookViews>
   <sheets>
     <sheet name="Página1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -141,8 +149,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -164,6 +172,10 @@
     <font>
       <b/>
       <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -324,7 +336,7 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
@@ -333,10 +345,10 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -347,7 +359,7 @@
         <color rgb="FF000000"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -355,13 +367,13 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -442,6 +454,10 @@
     <xf numFmtId="14" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -454,10 +470,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -776,39 +788,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="7.140625" customWidth="1"/>
-    <col min="2" max="2" width="41.140625" customWidth="1"/>
-    <col min="3" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.1640625" customWidth="1"/>
+    <col min="2" max="2" width="41.1640625" customWidth="1"/>
+    <col min="3" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A1" s="37" t="s">
+    <row r="1" spans="1:9" ht="13" x14ac:dyDescent="0.15">
+      <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="33" t="s">
+      <c r="B1" s="36"/>
+      <c r="C1" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="34"/>
-      <c r="E1" s="35" t="s">
+      <c r="D1" s="36"/>
+      <c r="E1" s="37" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="38" t="s">
+      <c r="G1" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="34"/>
-    </row>
-    <row r="2" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="H1" s="36"/>
+    </row>
+    <row r="2" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -821,7 +833,7 @@
       <c r="D2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="36"/>
+      <c r="E2" s="38"/>
       <c r="F2" s="5" t="s">
         <v>9</v>
       </c>
@@ -833,7 +845,7 @@
       </c>
       <c r="I2" s="7"/>
     </row>
-    <row r="3" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
         <v>11</v>
       </c>
@@ -853,7 +865,7 @@
       <c r="G3" s="22"/>
       <c r="H3" s="26"/>
     </row>
-    <row r="4" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A4" s="8" t="s">
         <v>13</v>
       </c>
@@ -869,11 +881,11 @@
       <c r="E4" s="8">
         <v>6</v>
       </c>
-      <c r="F4" s="40"/>
-      <c r="G4" s="39"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="33"/>
       <c r="H4" s="27"/>
     </row>
-    <row r="5" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A5" s="12" t="s">
         <v>15</v>
       </c>
@@ -889,11 +901,11 @@
       <c r="E5" s="8">
         <v>6</v>
       </c>
-      <c r="F5" s="40"/>
-      <c r="G5" s="39"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="33"/>
       <c r="H5" s="27"/>
     </row>
-    <row r="6" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A6" s="12" t="s">
         <v>17</v>
       </c>
@@ -913,7 +925,7 @@
       <c r="G6" s="25"/>
       <c r="H6" s="10"/>
     </row>
-    <row r="7" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A7" s="12" t="s">
         <v>19</v>
       </c>
@@ -927,7 +939,7 @@
       <c r="G7" s="15"/>
       <c r="H7" s="27"/>
     </row>
-    <row r="8" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A8" s="12" t="s">
         <v>21</v>
       </c>
@@ -941,7 +953,7 @@
       <c r="G8" s="15"/>
       <c r="H8" s="27"/>
     </row>
-    <row r="9" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A9" s="12" t="s">
         <v>23</v>
       </c>
@@ -954,7 +966,7 @@
       <c r="G9" s="15"/>
       <c r="H9" s="27"/>
     </row>
-    <row r="10" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A10" s="12" t="s">
         <v>25</v>
       </c>
@@ -968,7 +980,7 @@
       <c r="G10" s="15"/>
       <c r="H10" s="27"/>
     </row>
-    <row r="11" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A11" s="12" t="s">
         <v>27</v>
       </c>
@@ -982,7 +994,7 @@
       <c r="G11" s="21"/>
       <c r="H11" s="27"/>
     </row>
-    <row r="12" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A12" s="12" t="s">
         <v>29</v>
       </c>
@@ -996,7 +1008,7 @@
       <c r="G12" s="15"/>
       <c r="H12" s="14"/>
     </row>
-    <row r="13" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A13" s="12" t="s">
         <v>31</v>
       </c>
@@ -1010,7 +1022,7 @@
       <c r="G13" s="15"/>
       <c r="H13" s="14"/>
     </row>
-    <row r="14" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A14" s="12" t="s">
         <v>33</v>
       </c>
@@ -1024,7 +1036,7 @@
       <c r="G14" s="15"/>
       <c r="H14" s="14"/>
     </row>
-    <row r="15" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A15" s="12" t="s">
         <v>35</v>
       </c>
@@ -1038,7 +1050,7 @@
       <c r="G15" s="15"/>
       <c r="H15" s="14"/>
     </row>
-    <row r="16" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A16" s="16" t="s">
         <v>37</v>
       </c>
@@ -1052,7 +1064,7 @@
       <c r="G16" s="19"/>
       <c r="H16" s="18"/>
     </row>
-    <row r="17" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" ht="13" x14ac:dyDescent="0.15">
       <c r="A17" s="7"/>
     </row>
   </sheetData>
@@ -1062,6 +1074,8 @@
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="G1:H1"/>
   </mergeCells>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>